<commit_message>
- update getPVPowerprofile.py - method simulationsmodel as a function of design params - default solver GLPK
</commit_message>
<xml_diff>
--- a/Finesimulations/GRID_PV_Storage/Results/SourceSinkModel.xlsx
+++ b/Finesimulations/GRID_PV_Storage/Results/SourceSinkModel.xlsx
@@ -493,7 +493,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.6857895834986604</v>
+        <v>4041.375937365727</v>
       </c>
     </row>
     <row r="3">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.6857895834986597</v>
+        <v>4041.375937365723</v>
       </c>
     </row>
     <row r="4">
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.6857895834986597</v>
+        <v>4041.375937365723</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.959398809996169</v>
+        <v>11546.78839247327</v>
       </c>
     </row>
     <row r="7">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.959398809996169</v>
+        <v>11546.78839247327</v>
       </c>
     </row>
     <row r="8">
@@ -605,7 +605,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>949.8875726728809</v>
+        <v>2062.858975181512</v>
       </c>
     </row>
     <row r="10">
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>949.8875726728802</v>
+        <v>2062.85897518151</v>
       </c>
     </row>
     <row r="11">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>13.81414217987393</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>784.1178665143931</v>
+        <v>1702.85897518151</v>
       </c>
     </row>
     <row r="13">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>13.81414217987393</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>11051.31374389914</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="18">
@@ -765,7 +765,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>15302.01770925734</v>
+        <v>17835.43650000022</v>
       </c>
     </row>
     <row r="20">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>15302.01770925734</v>
+        <v>17835.43650000022</v>
       </c>
     </row>
     <row r="21">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>165.7697061584871</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>3112.629295829287</v>
+        <v>186262.6104983193</v>
       </c>
     </row>
     <row r="25">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3112.629295829285</v>
+        <v>186262.6104983191</v>
       </c>
     </row>
     <row r="26">
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>62.25258591658712</v>
+        <v>3725.252209966534</v>
       </c>
     </row>
     <row r="29">
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>62.25258591658712</v>
+        <v>3725.252209966534</v>
       </c>
     </row>
     <row r="30">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3112.629295829285</v>
+        <v>186262.6104983191</v>
       </c>
     </row>
     <row r="31">
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2021.759999999986</v>
+        <v>20217.59999999952</v>
       </c>
     </row>
     <row r="36">
@@ -1033,7 +1033,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2021.759999999986</v>
+        <v>20217.59999999952</v>
       </c>
     </row>
     <row r="37">
@@ -1069,7 +1069,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>-658.7571142139425</v>
+        <v>-452.7745246309626</v>
       </c>
     </row>
     <row r="39">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>-658.7571142139418</v>
+        <v>-452.7745246309621</v>
       </c>
     </row>
     <row r="40">
@@ -1117,7 +1117,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>658.7571142139418</v>
+        <v>452.7745246309621</v>
       </c>
     </row>
     <row r="42">
@@ -1133,7 +1133,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>13175.14228427892</v>
+        <v>9055.490492619159</v>
       </c>
     </row>
     <row r="43">
@@ -1145,7 +1145,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>13175.14228427892</v>
+        <v>9055.490492619159</v>
       </c>
     </row>
     <row r="44">

</xml_diff>